<commit_message>
Affect the pin out to the signal
</commit_message>
<xml_diff>
--- a/M20DX256 Eval Board/ressource/pin_out_mk20.xlsx
+++ b/M20DX256 Eval Board/ressource/pin_out_mk20.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="123">
   <si>
     <t>J2</t>
   </si>
@@ -298,6 +298,93 @@
   </si>
   <si>
     <t>ADC1 7</t>
+  </si>
+  <si>
+    <t>ESW3_RX</t>
+  </si>
+  <si>
+    <t>ESW3_TX</t>
+  </si>
+  <si>
+    <t>LCD_SDA</t>
+  </si>
+  <si>
+    <t>LCD_SCL</t>
+  </si>
+  <si>
+    <t>Wheel_0</t>
+  </si>
+  <si>
+    <t>Wheel_1</t>
+  </si>
+  <si>
+    <t>Wheel_1_Led_1</t>
+  </si>
+  <si>
+    <t>Wheel_1_Led_0</t>
+  </si>
+  <si>
+    <t>Wheel_0_Led_1</t>
+  </si>
+  <si>
+    <t>Wheel_0_Led_0</t>
+  </si>
+  <si>
+    <t>LED_1</t>
+  </si>
+  <si>
+    <t>LED_0</t>
+  </si>
+  <si>
+    <t>Direction_1</t>
+  </si>
+  <si>
+    <t>Direction_2</t>
+  </si>
+  <si>
+    <t>Push_button_1</t>
+  </si>
+  <si>
+    <t>Push_button_2</t>
+  </si>
+  <si>
+    <t>Joystick_D</t>
+  </si>
+  <si>
+    <t>Joystick_A</t>
+  </si>
+  <si>
+    <t>Joystick_B</t>
+  </si>
+  <si>
+    <t>Joystick_C</t>
+  </si>
+  <si>
+    <t>Joystick_Push</t>
+  </si>
+  <si>
+    <t>Encoder_A</t>
+  </si>
+  <si>
+    <t>Encoder_B</t>
+  </si>
+  <si>
+    <t>LCD_LED_0</t>
+  </si>
+  <si>
+    <t>LCD_LED_1</t>
+  </si>
+  <si>
+    <t>LCD_LED_2</t>
+  </si>
+  <si>
+    <t>LCD_LED_3</t>
+  </si>
+  <si>
+    <t>ESW3_TOR</t>
+  </si>
+  <si>
+    <t>PWM_LCD</t>
   </si>
 </sst>
 </file>
@@ -321,7 +408,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -553,11 +640,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -605,6 +701,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -906,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+      <selection activeCell="K19" sqref="K18:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,9 +1017,10 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -951,7 +1049,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -968,7 +1066,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="22"/>
       <c r="B3" s="1">
         <v>2</v>
@@ -988,8 +1086,11 @@
         <v>85</v>
       </c>
       <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
       <c r="B4" s="1">
         <v>3</v>
@@ -1009,8 +1110,11 @@
         <v>84</v>
       </c>
       <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
       <c r="B5" s="1">
         <v>4</v>
@@ -1026,8 +1130,11 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
       <c r="B6" s="1">
         <v>5</v>
@@ -1043,8 +1150,11 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="1">
         <v>6</v>
@@ -1062,8 +1172,11 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="1">
         <v>7</v>
@@ -1081,8 +1194,11 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="1">
         <v>8</v>
@@ -1102,8 +1218,11 @@
         <v>83</v>
       </c>
       <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="1">
         <v>9</v>
@@ -1123,8 +1242,11 @@
         <v>82</v>
       </c>
       <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="1">
         <v>10</v>
@@ -1144,8 +1266,11 @@
         <v>81</v>
       </c>
       <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="1">
         <v>11</v>
@@ -1165,8 +1290,11 @@
         <v>80</v>
       </c>
       <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="1">
         <v>12</v>
@@ -1180,8 +1308,11 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" s="1">
         <v>13</v>
@@ -1196,7 +1327,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="1">
         <v>14</v>
@@ -1213,7 +1344,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="8"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="1">
         <v>15</v>
@@ -1232,7 +1363,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
       <c r="B17" s="1">
         <v>16</v>
@@ -1247,7 +1378,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
       <c r="B18" s="1">
         <v>17</v>
@@ -1261,8 +1392,11 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="1">
         <v>18</v>
@@ -1276,8 +1410,11 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="8"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="1">
         <v>19</v>
@@ -1291,8 +1428,11 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="23"/>
       <c r="B21" s="10">
         <v>20</v>
@@ -1306,8 +1446,11 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="12"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>20</v>
       </c>
@@ -1329,8 +1472,11 @@
         <v>91</v>
       </c>
       <c r="I22" s="13"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
       <c r="B23" s="1">
         <v>2</v>
@@ -1350,8 +1496,11 @@
         <v>90</v>
       </c>
       <c r="I23" s="8"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
       <c r="B24" s="1">
         <v>3</v>
@@ -1368,7 +1517,7 @@
       </c>
       <c r="I24" s="8"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
       <c r="B25" s="1">
         <v>4</v>
@@ -1385,7 +1534,7 @@
       </c>
       <c r="I25" s="8"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
       <c r="B26" s="1">
         <v>5</v>
@@ -1399,8 +1548,11 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="8"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="1">
         <v>6</v>
@@ -1414,8 +1566,11 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="8"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="1">
         <v>7</v>
@@ -1429,8 +1584,11 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="8"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
       <c r="B29" s="1">
         <v>8</v>
@@ -1446,8 +1604,11 @@
         <v>87</v>
       </c>
       <c r="I29" s="8"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
       <c r="B30" s="1">
         <v>9</v>
@@ -1462,7 +1623,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="8"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
       <c r="B31" s="1">
         <v>10</v>
@@ -1480,8 +1641,11 @@
         <v>93</v>
       </c>
       <c r="I31" s="8"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
       <c r="B32" s="1">
         <v>11</v>
@@ -1499,8 +1663,11 @@
         <v>92</v>
       </c>
       <c r="I32" s="8"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
       <c r="B33" s="1">
         <v>12</v>
@@ -1516,8 +1683,11 @@
         <v>91</v>
       </c>
       <c r="I33" s="8"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
       <c r="B34" s="1">
         <v>13</v>
@@ -1533,8 +1703,11 @@
         <v>90</v>
       </c>
       <c r="I34" s="8"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
       <c r="B35" s="1">
         <v>14</v>
@@ -1550,8 +1723,11 @@
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="8"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
       <c r="B36" s="1">
         <v>15</v>
@@ -1567,8 +1743,11 @@
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="8"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
       <c r="B37" s="1">
         <v>16</v>
@@ -1584,8 +1763,11 @@
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="8"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
       <c r="B38" s="1">
         <v>17</v>
@@ -1602,7 +1784,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="8"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
       <c r="B39" s="1">
         <v>18</v>
@@ -1621,7 +1803,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="8"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
       <c r="B40" s="1">
         <v>19</v>
@@ -1642,7 +1824,7 @@
       </c>
       <c r="I40" s="8"/>
     </row>
-    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="24"/>
       <c r="B41" s="5">
         <v>20</v>
@@ -1656,6 +1838,9 @@
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="I41" s="9"/>
+      <c r="J41" t="s">
+        <v>122</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Affect pinout to varmo
</commit_message>
<xml_diff>
--- a/M20DX256 Eval Board/ressource/pin_out_mk20.xlsx
+++ b/M20DX256 Eval Board/ressource/pin_out_mk20.xlsx
@@ -306,12 +306,6 @@
     <t>ESW3_TX</t>
   </si>
   <si>
-    <t>LCD_SDA</t>
-  </si>
-  <si>
-    <t>LCD_SCL</t>
-  </si>
-  <si>
     <t>Wheel_0</t>
   </si>
   <si>
@@ -333,58 +327,64 @@
     <t>LED_1</t>
   </si>
   <si>
-    <t>LED_0</t>
-  </si>
-  <si>
-    <t>Direction_1</t>
-  </si>
-  <si>
-    <t>Direction_2</t>
-  </si>
-  <si>
-    <t>Push_button_1</t>
-  </si>
-  <si>
-    <t>Push_button_2</t>
-  </si>
-  <si>
-    <t>Joystick_D</t>
-  </si>
-  <si>
-    <t>Joystick_A</t>
-  </si>
-  <si>
-    <t>Joystick_B</t>
-  </si>
-  <si>
-    <t>Joystick_C</t>
-  </si>
-  <si>
-    <t>Joystick_Push</t>
-  </si>
-  <si>
-    <t>Encoder_A</t>
-  </si>
-  <si>
-    <t>Encoder_B</t>
-  </si>
-  <si>
-    <t>LCD_LED_0</t>
-  </si>
-  <si>
-    <t>LCD_LED_1</t>
-  </si>
-  <si>
-    <t>LCD_LED_2</t>
-  </si>
-  <si>
-    <t>LCD_LED_3</t>
-  </si>
-  <si>
     <t>ESW3_TOR</t>
   </si>
   <si>
-    <t>PWM_LCD</t>
+    <t>LED_STATUS_1</t>
+  </si>
+  <si>
+    <t>LED_STATUS_2</t>
+  </si>
+  <si>
+    <t>LED_STATUS_3</t>
+  </si>
+  <si>
+    <t>LED_STATUS_4</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>DIR_A</t>
+  </si>
+  <si>
+    <t>DIR_B</t>
+  </si>
+  <si>
+    <t>DIR_C</t>
+  </si>
+  <si>
+    <t>DIR_D</t>
+  </si>
+  <si>
+    <t>ENCODER_A</t>
+  </si>
+  <si>
+    <t>ENCODER_B</t>
+  </si>
+  <si>
+    <t>PUSH</t>
+  </si>
+  <si>
+    <t>LED_2</t>
+  </si>
+  <si>
+    <t>PUSH_BUTTON_2</t>
+  </si>
+  <si>
+    <t>PUSH_BUTTON_1</t>
+  </si>
+  <si>
+    <t>DIRECTION_1</t>
+  </si>
+  <si>
+    <t>DIRECTION_2</t>
+  </si>
+  <si>
+    <t>PWM_CONTRASTE</t>
   </si>
 </sst>
 </file>
@@ -400,12 +400,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="18">
@@ -653,7 +659,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -701,7 +707,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1005,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K19" sqref="K18:K19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,7 +1024,8 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1086,8 +1094,8 @@
         <v>85</v>
       </c>
       <c r="I3" s="8"/>
-      <c r="J3" t="s">
-        <v>103</v>
+      <c r="J3" s="25" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1110,8 +1118,8 @@
         <v>84</v>
       </c>
       <c r="I4" s="8"/>
-      <c r="J4" t="s">
-        <v>102</v>
+      <c r="J4" s="25" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1130,8 +1138,8 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="8"/>
-      <c r="J5" t="s">
-        <v>101</v>
+      <c r="J5" s="25" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1150,8 +1158,8 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="8"/>
-      <c r="J6" t="s">
-        <v>100</v>
+      <c r="J6" s="25" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1172,7 +1180,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="8"/>
-      <c r="J7" t="s">
+      <c r="J7" s="25" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1194,7 +1202,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="8"/>
-      <c r="J8" t="s">
+      <c r="J8" s="25" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1218,8 +1226,8 @@
         <v>83</v>
       </c>
       <c r="I9" s="8"/>
-      <c r="J9" t="s">
-        <v>98</v>
+      <c r="J9" s="25" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1242,8 +1250,8 @@
         <v>82</v>
       </c>
       <c r="I10" s="8"/>
-      <c r="J10" t="s">
-        <v>99</v>
+      <c r="J10" s="25" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1266,8 +1274,8 @@
         <v>81</v>
       </c>
       <c r="I11" s="8"/>
-      <c r="J11" t="s">
-        <v>96</v>
+      <c r="J11" s="25" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1290,8 +1298,8 @@
         <v>80</v>
       </c>
       <c r="I12" s="8"/>
-      <c r="J12" t="s">
-        <v>97</v>
+      <c r="J12" s="25" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1308,8 +1316,8 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="8"/>
-      <c r="J13" t="s">
-        <v>121</v>
+      <c r="J13" s="25" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1326,6 +1334,9 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="8"/>
+      <c r="J14" s="25" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
@@ -1392,9 +1403,6 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="8"/>
-      <c r="J18" t="s">
-        <v>117</v>
-      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
@@ -1410,9 +1418,6 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="8"/>
-      <c r="J19" t="s">
-        <v>118</v>
-      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
@@ -1428,9 +1433,6 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="8"/>
-      <c r="J20" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="23"/>
@@ -1446,9 +1448,6 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="12"/>
-      <c r="J21" t="s">
-        <v>120</v>
-      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
@@ -1473,7 +1472,7 @@
       </c>
       <c r="I22" s="13"/>
       <c r="J22" s="25" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1497,7 +1496,7 @@
       </c>
       <c r="I23" s="8"/>
       <c r="J23" s="25" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1516,6 +1515,9 @@
         <v>89</v>
       </c>
       <c r="I24" s="8"/>
+      <c r="J24" s="25" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
@@ -1533,6 +1535,9 @@
         <v>88</v>
       </c>
       <c r="I25" s="8"/>
+      <c r="J25" s="25" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
@@ -1548,8 +1553,8 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="8"/>
-      <c r="J26" t="s">
-        <v>106</v>
+      <c r="J26" s="26" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1566,8 +1571,8 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="8"/>
-      <c r="J27" t="s">
-        <v>107</v>
+      <c r="J27" s="26" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1584,9 +1589,6 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="8"/>
-      <c r="J28" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
@@ -1604,8 +1606,8 @@
         <v>87</v>
       </c>
       <c r="I29" s="8"/>
-      <c r="J29" t="s">
-        <v>109</v>
+      <c r="J29" s="25" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1622,6 +1624,9 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="8"/>
+      <c r="J30" s="25" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
@@ -1641,8 +1646,8 @@
         <v>93</v>
       </c>
       <c r="I31" s="8"/>
-      <c r="J31" t="s">
-        <v>115</v>
+      <c r="J31" s="25" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1663,8 +1668,8 @@
         <v>92</v>
       </c>
       <c r="I32" s="8"/>
-      <c r="J32" t="s">
-        <v>116</v>
+      <c r="J32" s="25" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1683,7 +1688,7 @@
         <v>91</v>
       </c>
       <c r="I33" s="8"/>
-      <c r="J33" t="s">
+      <c r="J33" s="25" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1703,8 +1708,8 @@
         <v>90</v>
       </c>
       <c r="I34" s="8"/>
-      <c r="J34" t="s">
-        <v>111</v>
+      <c r="J34" s="25" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1723,8 +1728,8 @@
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="8"/>
-      <c r="J35" t="s">
-        <v>112</v>
+      <c r="J35" s="25" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -1743,9 +1748,6 @@
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="8"/>
-      <c r="J36" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
@@ -1763,8 +1765,8 @@
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="8"/>
-      <c r="J37" t="s">
-        <v>110</v>
+      <c r="J37" s="25" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -1783,6 +1785,9 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="8"/>
+      <c r="J38" s="25" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
@@ -1802,6 +1807,9 @@
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="8"/>
+      <c r="J39" s="25" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
@@ -1823,6 +1831,9 @@
         <v>86</v>
       </c>
       <c r="I40" s="8"/>
+      <c r="J40" s="25" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="24"/>
@@ -1838,9 +1849,6 @@
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="I41" s="9"/>
-      <c r="J41" t="s">
-        <v>122</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1848,6 +1856,7 @@
     <mergeCell ref="A22:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>